<commit_message>
0.1.5: Not describe Object.assign for toJSON method, if super class has no properties.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectTsClassStructure.xlsx
+++ b/meta/program/BlancoValueObjectTsClassStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCD71AD-240C-B14D-9602-69B9341E0E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06119B90-7CE6-4A45-BFF4-289BEADCE7FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10100" yWindow="920" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="94">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -480,6 +480,17 @@
     </rPh>
     <rPh sb="65" eb="67">
       <t xml:space="preserve">シヨウシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>generateToJson</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>toJSONメソッドを生成するかどうか。このフラグはant taskのオプションとして供給される。</t>
+    <rPh sb="43" eb="45">
+      <t xml:space="preserve">キョウキュウ </t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -1015,47 +1026,47 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1467,10 +1478,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:F30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1665,24 +1676,24 @@
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="52"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="54"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="52"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="54"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -1724,30 +1735,30 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="53" t="s">
+      <c r="C25" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="53" t="s">
+      <c r="D25" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="53" t="s">
+      <c r="E25" s="48" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="58"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
       <c r="F26" s="9"/>
       <c r="G26"/>
     </row>
@@ -1788,7 +1799,7 @@
     </row>
     <row r="29" spans="1:7" ht="47" customHeight="1">
       <c r="A29" s="38">
-        <f t="shared" ref="A29:A49" si="0">A28+1</f>
+        <f t="shared" ref="A29:A50" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="39" t="s">
@@ -1798,10 +1809,10 @@
         <v>33</v>
       </c>
       <c r="D29" s="40"/>
-      <c r="E29" s="56" t="s">
+      <c r="E29" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="57"/>
+      <c r="F29" s="58"/>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7" ht="47" customHeight="1">
@@ -1816,10 +1827,10 @@
         <v>33</v>
       </c>
       <c r="D30" s="40"/>
-      <c r="E30" s="56" t="s">
+      <c r="E30" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="57"/>
+      <c r="F30" s="58"/>
       <c r="G30"/>
     </row>
     <row r="31" spans="1:7" ht="15">
@@ -1854,10 +1865,10 @@
       <c r="D32" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="F32" s="50"/>
+      <c r="F32" s="52"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="15">
@@ -1874,10 +1885,10 @@
       <c r="D33" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="F33" s="50"/>
+      <c r="F33" s="52"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="15">
@@ -1894,10 +1905,10 @@
       <c r="D34" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="49" t="s">
+      <c r="E34" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="F34" s="50"/>
+      <c r="F34" s="52"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="15">
@@ -1914,10 +1925,10 @@
       <c r="D35" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="54" t="s">
+      <c r="E35" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="F35" s="55"/>
+      <c r="F35" s="56"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" ht="15">
@@ -1934,10 +1945,10 @@
       <c r="D36" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="49" t="s">
+      <c r="E36" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="50"/>
+      <c r="F36" s="52"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" ht="15">
@@ -1954,10 +1965,10 @@
       <c r="D37" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="49" t="s">
+      <c r="E37" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="F37" s="50"/>
+      <c r="F37" s="52"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" ht="15">
@@ -1974,10 +1985,10 @@
       <c r="D38" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="49" t="s">
+      <c r="E38" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="F38" s="50"/>
+      <c r="F38" s="52"/>
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7" ht="15">
@@ -1994,10 +2005,10 @@
       <c r="D39" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="49" t="s">
+      <c r="E39" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="50"/>
+      <c r="F39" s="52"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" ht="15">
@@ -2014,10 +2025,10 @@
       <c r="D40" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="49" t="s">
+      <c r="E40" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="F40" s="50"/>
+      <c r="F40" s="52"/>
       <c r="G40"/>
     </row>
     <row r="41" spans="1:7" ht="15">
@@ -2034,10 +2045,10 @@
       <c r="D41" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E41" s="49" t="s">
+      <c r="E41" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="F41" s="50"/>
+      <c r="F41" s="52"/>
       <c r="G41"/>
     </row>
     <row r="42" spans="1:7" ht="15">
@@ -2054,10 +2065,10 @@
       <c r="D42" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="49" t="s">
+      <c r="E42" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="50"/>
+      <c r="F42" s="52"/>
       <c r="G42"/>
     </row>
     <row r="43" spans="1:7" ht="15">
@@ -2074,10 +2085,10 @@
       <c r="D43" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="49" t="s">
+      <c r="E43" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="F43" s="50"/>
+      <c r="F43" s="52"/>
       <c r="G43"/>
     </row>
     <row r="44" spans="1:7" ht="15">
@@ -2094,10 +2105,10 @@
       <c r="D44" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="49" t="s">
+      <c r="E44" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="F44" s="50"/>
+      <c r="F44" s="52"/>
       <c r="G44"/>
     </row>
     <row r="45" spans="1:7" ht="15">
@@ -2112,10 +2123,10 @@
         <v>33</v>
       </c>
       <c r="D45" s="40"/>
-      <c r="E45" s="49" t="s">
+      <c r="E45" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="F45" s="50"/>
+      <c r="F45" s="52"/>
       <c r="G45"/>
     </row>
     <row r="46" spans="1:7" ht="45" customHeight="1">
@@ -2132,10 +2143,10 @@
       <c r="D46" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E46" s="49" t="s">
+      <c r="E46" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="F46" s="51"/>
+      <c r="F46" s="53"/>
       <c r="G46"/>
     </row>
     <row r="47" spans="1:7" ht="45">
@@ -2152,10 +2163,10 @@
       <c r="D47" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="E47" s="49" t="s">
+      <c r="E47" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="F47" s="51"/>
+      <c r="F47" s="53"/>
       <c r="G47"/>
     </row>
     <row r="48" spans="1:7" ht="15">
@@ -2170,10 +2181,10 @@
         <v>63</v>
       </c>
       <c r="D48" s="40"/>
-      <c r="E48" s="49" t="s">
+      <c r="E48" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="F48" s="51"/>
+      <c r="F48" s="53"/>
       <c r="G48"/>
     </row>
     <row r="49" spans="1:7">
@@ -2190,34 +2201,58 @@
       <c r="D49" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="E49" s="49" t="s">
+      <c r="E49" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="F49" s="50"/>
+      <c r="F49" s="52"/>
       <c r="G49"/>
     </row>
-    <row r="50" spans="1:7" ht="14" customHeight="1">
-      <c r="A50" s="21"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="48"/>
+    <row r="50" spans="1:7" ht="15">
+      <c r="A50" s="38">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B50" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="F50" s="52"/>
       <c r="G50"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" ht="14" customHeight="1">
+      <c r="A51" s="21"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="60"/>
       <c r="G51"/>
     </row>
+    <row r="52" spans="1:7">
+      <c r="G52"/>
+    </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
+  <mergeCells count="32">
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E49:F49"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="E19:E20"/>
@@ -2230,21 +2265,18 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D64" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D65" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
0.1.9: Implent label option. if label is true, fields are declared public and methods are not generated.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectTsClassStructure.xlsx
+++ b/meta/program/BlancoValueObjectTsClassStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5887C0-177D-1541-B504-33B175C20488}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB143C0-D1C2-F24D-B773-BE59AA7E97C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10100" yWindow="920" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="98">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -522,6 +522,20 @@
       <t xml:space="preserve">スベテノ </t>
     </rPh>
     <rPh sb="56" eb="58">
+      <t xml:space="preserve">ユウセｎ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>label</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ラベル定義用かどうか。通常は false。インタフェイス指定があればそちらが優先します。</t>
+    <rPh sb="28" eb="30">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="38" eb="40">
       <t xml:space="preserve">ユウセｎ </t>
     </rPh>
     <phoneticPr fontId="3"/>
@@ -1058,47 +1072,47 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1510,10 +1524,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52:F52"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1708,24 +1722,24 @@
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="52"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="54"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="52"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="54"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -1767,30 +1781,30 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="53" t="s">
+      <c r="C25" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="53" t="s">
+      <c r="D25" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="53" t="s">
+      <c r="E25" s="48" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="58"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
       <c r="F26" s="9"/>
       <c r="G26"/>
     </row>
@@ -1831,7 +1845,7 @@
     </row>
     <row r="29" spans="1:7" ht="47" customHeight="1">
       <c r="A29" s="38">
-        <f t="shared" ref="A29:A51" si="0">A28+1</f>
+        <f t="shared" ref="A29:A52" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="39" t="s">
@@ -1841,10 +1855,10 @@
         <v>33</v>
       </c>
       <c r="D29" s="40"/>
-      <c r="E29" s="56" t="s">
+      <c r="E29" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="57"/>
+      <c r="F29" s="58"/>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7" ht="47" customHeight="1">
@@ -1859,10 +1873,10 @@
         <v>33</v>
       </c>
       <c r="D30" s="40"/>
-      <c r="E30" s="56" t="s">
+      <c r="E30" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="57"/>
+      <c r="F30" s="58"/>
       <c r="G30"/>
     </row>
     <row r="31" spans="1:7" ht="15">
@@ -1897,10 +1911,10 @@
       <c r="D32" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="F32" s="50"/>
+      <c r="F32" s="52"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="15">
@@ -1917,10 +1931,10 @@
       <c r="D33" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="F33" s="50"/>
+      <c r="F33" s="52"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="15">
@@ -1937,10 +1951,10 @@
       <c r="D34" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="49" t="s">
+      <c r="E34" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="F34" s="50"/>
+      <c r="F34" s="52"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="15">
@@ -1957,10 +1971,10 @@
       <c r="D35" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="54" t="s">
+      <c r="E35" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="F35" s="55"/>
+      <c r="F35" s="56"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" ht="15">
@@ -1977,10 +1991,10 @@
       <c r="D36" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="49" t="s">
+      <c r="E36" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="50"/>
+      <c r="F36" s="52"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" ht="15">
@@ -1997,10 +2011,10 @@
       <c r="D37" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="49" t="s">
+      <c r="E37" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="F37" s="50"/>
+      <c r="F37" s="52"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" ht="15">
@@ -2017,10 +2031,10 @@
       <c r="D38" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="49" t="s">
+      <c r="E38" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="F38" s="50"/>
+      <c r="F38" s="52"/>
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7" ht="15">
@@ -2037,10 +2051,10 @@
       <c r="D39" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="49" t="s">
+      <c r="E39" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="50"/>
+      <c r="F39" s="52"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" ht="15">
@@ -2057,10 +2071,10 @@
       <c r="D40" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="49" t="s">
+      <c r="E40" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="F40" s="50"/>
+      <c r="F40" s="52"/>
       <c r="G40"/>
     </row>
     <row r="41" spans="1:7" ht="15">
@@ -2069,18 +2083,18 @@
         <v>15</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C41" s="40" t="s">
         <v>77</v>
       </c>
       <c r="D41" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="E41" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="F41" s="50"/>
+        <v>42</v>
+      </c>
+      <c r="E41" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="F41" s="52"/>
       <c r="G41"/>
     </row>
     <row r="42" spans="1:7" ht="15">
@@ -2089,7 +2103,7 @@
         <v>16</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C42" s="40" t="s">
         <v>77</v>
@@ -2097,10 +2111,10 @@
       <c r="D42" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="F42" s="50"/>
+      <c r="E42" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" s="52"/>
       <c r="G42"/>
     </row>
     <row r="43" spans="1:7" ht="15">
@@ -2109,7 +2123,7 @@
         <v>17</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C43" s="40" t="s">
         <v>77</v>
@@ -2117,10 +2131,10 @@
       <c r="D43" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="F43" s="50"/>
+      <c r="E43" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" s="52"/>
       <c r="G43"/>
     </row>
     <row r="44" spans="1:7" ht="15">
@@ -2129,7 +2143,7 @@
         <v>18</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C44" s="40" t="s">
         <v>77</v>
@@ -2137,10 +2151,10 @@
       <c r="D44" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="F44" s="50"/>
+      <c r="E44" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" s="52"/>
       <c r="G44"/>
     </row>
     <row r="45" spans="1:7" ht="15">
@@ -2149,114 +2163,114 @@
         <v>19</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="40"/>
-      <c r="E45" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="F45" s="50"/>
+        <v>77</v>
+      </c>
+      <c r="D45" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45" s="52"/>
       <c r="G45"/>
     </row>
-    <row r="46" spans="1:7" ht="45" customHeight="1">
+    <row r="46" spans="1:7" ht="15">
       <c r="A46" s="38">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="E46" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="F46" s="51"/>
+        <v>33</v>
+      </c>
+      <c r="D46" s="40"/>
+      <c r="E46" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="F46" s="52"/>
       <c r="G46"/>
     </row>
-    <row r="47" spans="1:7" ht="45">
+    <row r="47" spans="1:7" ht="45" customHeight="1">
       <c r="A47" s="38">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="D47" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="E47" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47" s="51"/>
+        <v>57</v>
+      </c>
+      <c r="E47" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" s="53"/>
       <c r="G47"/>
     </row>
-    <row r="48" spans="1:7" ht="15">
+    <row r="48" spans="1:7" ht="45">
       <c r="A48" s="38">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="40"/>
-      <c r="E48" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="F48" s="51"/>
+        <v>80</v>
+      </c>
+      <c r="D48" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="E48" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="F48" s="53"/>
       <c r="G48"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" ht="15">
       <c r="A49" s="38">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B49" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="C49" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="D49" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="E49" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="F49" s="50"/>
+      <c r="B49" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="40"/>
+      <c r="E49" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="F49" s="53"/>
       <c r="G49"/>
     </row>
-    <row r="50" spans="1:7" ht="15">
+    <row r="50" spans="1:7">
       <c r="A50" s="38">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B50" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="D50" s="40" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="F50" s="50"/>
+      <c r="B50" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" s="52"/>
       <c r="G50"/>
     </row>
     <row r="51" spans="1:7" ht="15">
@@ -2265,7 +2279,7 @@
         <v>25</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C51" s="40" t="s">
         <v>77</v>
@@ -2273,26 +2287,72 @@
       <c r="D51" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="E51" s="49" t="s">
+      <c r="E51" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="52"/>
+      <c r="G51"/>
+    </row>
+    <row r="52" spans="1:7" ht="15">
+      <c r="A52" s="38">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B52" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="F51" s="50"/>
-      <c r="G51"/>
-    </row>
-    <row r="52" spans="1:7" ht="14" customHeight="1">
-      <c r="A52" s="21"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="48"/>
+      <c r="F52" s="52"/>
       <c r="G52"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" ht="14" customHeight="1">
+      <c r="A53" s="21"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="60"/>
       <c r="G53"/>
     </row>
+    <row r="54" spans="1:7">
+      <c r="G54"/>
+    </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E29:F29"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
@@ -2301,35 +2361,10 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D66" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D67" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
0.1.10: Support Enum class.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectTsClassStructure.xlsx
+++ b/meta/program/BlancoValueObjectTsClassStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB143C0-D1C2-F24D-B773-BE59AA7E97C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550D7B67-9FDB-894E-B618-4760B1C129D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10100" yWindow="920" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -536,6 +536,20 @@
       <t xml:space="preserve">シテイ </t>
     </rPh>
     <rPh sb="38" eb="40">
+      <t xml:space="preserve">ユウセｎ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>enumeration</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>列挙型かどうか。通常は false。インタフェイスかどうかよりも優先されます。</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">レッキョガタ </t>
+    </rPh>
+    <rPh sb="32" eb="34">
       <t xml:space="preserve">ユウセｎ </t>
     </rPh>
     <phoneticPr fontId="3"/>
@@ -1524,10 +1538,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:F42"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1845,7 +1859,7 @@
     </row>
     <row r="29" spans="1:7" ht="47" customHeight="1">
       <c r="A29" s="38">
-        <f t="shared" ref="A29:A52" si="0">A28+1</f>
+        <f t="shared" ref="A29:A53" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="39" t="s">
@@ -2083,7 +2097,7 @@
         <v>15</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C41" s="40" t="s">
         <v>77</v>
@@ -2092,7 +2106,7 @@
         <v>42</v>
       </c>
       <c r="E41" s="51" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F41" s="52"/>
       <c r="G41"/>
@@ -2103,16 +2117,16 @@
         <v>16</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="C42" s="40" t="s">
         <v>77</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E42" s="51" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="F42" s="52"/>
       <c r="G42"/>
@@ -2123,7 +2137,7 @@
         <v>17</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C43" s="40" t="s">
         <v>77</v>
@@ -2132,7 +2146,7 @@
         <v>45</v>
       </c>
       <c r="E43" s="51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F43" s="52"/>
       <c r="G43"/>
@@ -2143,7 +2157,7 @@
         <v>18</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C44" s="40" t="s">
         <v>77</v>
@@ -2152,7 +2166,7 @@
         <v>45</v>
       </c>
       <c r="E44" s="51" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="F44" s="52"/>
       <c r="G44"/>
@@ -2163,7 +2177,7 @@
         <v>19</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="C45" s="40" t="s">
         <v>77</v>
@@ -2172,7 +2186,7 @@
         <v>45</v>
       </c>
       <c r="E45" s="51" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="F45" s="52"/>
       <c r="G45"/>
@@ -2183,112 +2197,112 @@
         <v>20</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="40"/>
+        <v>77</v>
+      </c>
+      <c r="D46" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="E46" s="51" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="F46" s="52"/>
       <c r="G46"/>
     </row>
-    <row r="47" spans="1:7" ht="45" customHeight="1">
+    <row r="47" spans="1:7" ht="15">
       <c r="A47" s="38">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47" s="40" t="s">
-        <v>57</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D47" s="40"/>
       <c r="E47" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="F47" s="53"/>
+        <v>51</v>
+      </c>
+      <c r="F47" s="52"/>
       <c r="G47"/>
     </row>
-    <row r="48" spans="1:7" ht="45">
+    <row r="48" spans="1:7" ht="45" customHeight="1">
       <c r="A48" s="38">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="E48" s="51" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F48" s="53"/>
       <c r="G48"/>
     </row>
-    <row r="49" spans="1:7" ht="15">
+    <row r="49" spans="1:7" ht="45">
       <c r="A49" s="38">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" s="40"/>
+        <v>80</v>
+      </c>
+      <c r="D49" s="40" t="s">
+        <v>81</v>
+      </c>
       <c r="E49" s="51" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F49" s="53"/>
       <c r="G49"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" ht="15">
       <c r="A50" s="38">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B50" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="D50" s="46" t="s">
-        <v>73</v>
-      </c>
+      <c r="B50" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="40"/>
       <c r="E50" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="F50" s="52"/>
+        <v>62</v>
+      </c>
+      <c r="F50" s="53"/>
       <c r="G50"/>
     </row>
-    <row r="51" spans="1:7" ht="15">
+    <row r="51" spans="1:7">
       <c r="A51" s="38">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B51" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="D51" s="40" t="b">
-        <v>0</v>
+      <c r="B51" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="46" t="s">
+        <v>73</v>
       </c>
       <c r="E51" s="51" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="F51" s="52"/>
       <c r="G51"/>
@@ -2299,7 +2313,7 @@
         <v>26</v>
       </c>
       <c r="B52" s="39" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C52" s="40" t="s">
         <v>77</v>
@@ -2308,44 +2322,64 @@
         <v>0</v>
       </c>
       <c r="E52" s="51" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F52" s="52"/>
       <c r="G52"/>
     </row>
-    <row r="53" spans="1:7" ht="14" customHeight="1">
-      <c r="A53" s="21"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="59"/>
-      <c r="F53" s="60"/>
+    <row r="53" spans="1:7" ht="15">
+      <c r="A53" s="38">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B53" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D53" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="F53" s="52"/>
       <c r="G53"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" ht="14" customHeight="1">
+      <c r="A54" s="21"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="59"/>
+      <c r="F54" s="60"/>
       <c r="G54"/>
     </row>
+    <row r="55" spans="1:7">
+      <c r="G55"/>
+    </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="E53:F53"/>
+  <mergeCells count="35">
+    <mergeCell ref="E54:F54"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E41:F41"/>
     <mergeCell ref="E42:F42"/>
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E50:F50"/>
     <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E51:F51"/>
     <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
     <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E37:F37"/>
@@ -2353,6 +2387,7 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E40:F40"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
@@ -2364,7 +2399,7 @@
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D67" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D68" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>